<commit_message>
teste do nivel xNome
</commit_message>
<xml_diff>
--- a/dados_nfe.xlsx
+++ b/dados_nfe.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,11 @@
           <t>xMotivo</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>xNome</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -492,6 +497,11 @@
       <c r="G2" t="inlineStr">
         <is>
           <t>Autorizado o uso da NF-e</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>CAFE RANCHEIRO AGRO INDUSTRIAL LTDA</t>
         </is>
       </c>
     </row>

</xml_diff>